<commit_message>
working on cutting down the ms
</commit_message>
<xml_diff>
--- a/denguePaper/analysis/tables/InfectionModels.xlsx
+++ b/denguePaper/analysis/tables/InfectionModels.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t>Body</t>
   </si>
@@ -89,9 +89,6 @@
     <t>0.354</t>
   </si>
   <si>
-    <t>VC</t>
-  </si>
-  <si>
     <t>survival</t>
   </si>
   <si>
@@ -183,6 +180,57 @@
   </si>
   <si>
     <t>14.927</t>
+  </si>
+  <si>
+    <t>VC (no COE)</t>
+  </si>
+  <si>
+    <t>VC (COE)</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>0.979</t>
+  </si>
+  <si>
+    <t>1.172</t>
+  </si>
+  <si>
+    <t>0.280</t>
+  </si>
+  <si>
+    <t>0.288</t>
+  </si>
+  <si>
+    <t>0.866</t>
+  </si>
+  <si>
+    <t>0.445</t>
+  </si>
+  <si>
+    <t>0.801</t>
+  </si>
+  <si>
+    <t>35.844</t>
+  </si>
+  <si>
+    <t>3.548</t>
+  </si>
+  <si>
+    <t>0.1696</t>
+  </si>
+  <si>
+    <t>8.474</t>
+  </si>
+  <si>
+    <t>4.648</t>
+  </si>
+  <si>
+    <t>0.779 (0.168)</t>
+  </si>
+  <si>
+    <t>3.803 (0.449)</t>
   </si>
 </sst>
 </file>
@@ -498,15 +546,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="28" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -517,7 +567,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -584,13 +634,13 @@
         <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>12</v>
@@ -625,13 +675,13 @@
         <v>8</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>14</v>
@@ -666,13 +716,13 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>17</v>
@@ -686,68 +736,104 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>3.61E-2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>61.128999999999998</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1">
-        <v>5.891</v>
-      </c>
-      <c r="J8" s="1">
-        <v>5.2600000000000001E-2</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L8" s="1">
-        <v>8.0890000000000004</v>
-      </c>
-      <c r="M8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
       <c r="C9" s="1">
-        <v>3.847</v>
+        <v>3.61E-2</v>
       </c>
       <c r="D9" s="1">
-        <v>0.14610000000000001</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1">
-        <v>597.51</v>
+        <v>61.128999999999998</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>8</v>
@@ -756,16 +842,16 @@
         <v>2</v>
       </c>
       <c r="I9" s="1">
-        <v>3.1080000000000001</v>
+        <v>5.891</v>
       </c>
       <c r="J9" s="1">
-        <v>0.2114</v>
+        <v>5.2600000000000001E-2</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
+      </c>
+      <c r="L9" s="1">
+        <v>8.0890000000000004</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>8</v>
@@ -773,83 +859,124 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3.847</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.14610000000000001</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>597.51</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>8</v>
+        <v>8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3.1080000000000001</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.2114</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M11" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>